<commit_message>
Now handles trailing rows
</commit_message>
<xml_diff>
--- a/test1in.xlsx
+++ b/test1in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
-  <si>
-    <t xml:space="preserve">Example Table1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">Example TableOld</t>
   </si>
   <si>
     <t xml:space="preserve">Test by running: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out=test1out.xlsx</t>
@@ -80,7 +80,10 @@
     <t xml:space="preserve">orange</t>
   </si>
   <si>
-    <t xml:space="preserve">Example Table2</t>
+    <t xml:space="preserve">Trailing row here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example TableNew</t>
   </si>
   <si>
     <t xml:space="preserve">Shape</t>
@@ -230,8 +233,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,6 +339,9 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="F10" s="4"/>
     </row>
   </sheetData>
@@ -356,7 +362,7 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -364,7 +370,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,7 +386,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -391,13 +397,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,10 +411,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -422,7 +428,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Fixed bug: new data not shown when rows match
</commit_message>
<xml_diff>
--- a/test1in.xlsx
+++ b/test1in.xlsx
@@ -363,7 +363,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,7 +394,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
added --append and --merge options
</commit_message>
<xml_diff>
--- a/test1in.xlsx
+++ b/test1in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t xml:space="preserve">Example TableOld</t>
   </si>
@@ -77,34 +77,34 @@
     <t xml:space="preserve">Thailand</t>
   </si>
   <si>
+    <t xml:space="preserve">Trailing row here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example TableNew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grapes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pebbles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flat</t>
+  </si>
+  <si>
     <t xml:space="preserve">orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trailing row here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example TableNew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grapes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pebbles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mango</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flat</t>
   </si>
 </sst>
 </file>
@@ -233,11 +233,11 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -330,17 +330,15 @@
       <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>19</v>
+      <c r="A10" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -362,15 +360,15 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="E8 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,7 +384,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -397,13 +395,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,10 +409,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -428,10 +426,10 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E7" s="2"/>
     </row>

</xml_diff>

<commit_message>
Retain cell format with --merge option
</commit_message>
<xml_diff>
--- a/test1in.xlsx
+++ b/test1in.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t xml:space="preserve">Example TableOld</t>
   </si>
@@ -53,6 +53,15 @@
     <t xml:space="preserve">red</t>
   </si>
   <si>
+    <t xml:space="preserve">papaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pink</t>
+  </si>
+  <si>
     <t xml:space="preserve">banana</t>
   </si>
   <si>
@@ -105,6 +114,12 @@
   </si>
   <si>
     <t xml:space="preserve">orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elongated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salmon</t>
   </si>
 </sst>
 </file>
@@ -231,13 +246,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -285,10 +300,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
-        <v>44870</v>
+        <v>44867</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -302,10 +317,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
-        <v>44885</v>
+        <v>44870</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
@@ -319,10 +334,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>44886</v>
+        <v>44885</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -330,17 +345,34 @@
       <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="4"/>
+      <c r="A9" s="3" t="n">
+        <v>44886</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -361,14 +393,14 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="E8 A6"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,7 +416,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -395,13 +427,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,13 +441,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,17 +455,29 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added more rows to test data
</commit_message>
<xml_diff>
--- a/test1in.xlsx
+++ b/test1in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t xml:space="preserve">Example TableOld</t>
   </si>
   <si>
-    <t xml:space="preserve">Test by running: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out=test1out.xlsx</t>
+    <t xml:space="preserve">Diff test: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --out test1diff.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge test: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --merge=Color --out test1merge.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apend test: ./xltablediff.py --newSheet=Sheet2 --key=ID test1in.xlsx test1in.xlsx --append --out test1append.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
@@ -44,6 +50,15 @@
     <t xml:space="preserve">Color</t>
   </si>
   <si>
+    <t xml:space="preserve">apricot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red-orange</t>
+  </si>
+  <si>
     <t xml:space="preserve">apple</t>
   </si>
   <si>
@@ -53,6 +68,15 @@
     <t xml:space="preserve">red</t>
   </si>
   <si>
+    <t xml:space="preserve">peach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow-pink</t>
+  </si>
+  <si>
     <t xml:space="preserve">papaya</t>
   </si>
   <si>
@@ -62,6 +86,15 @@
     <t xml:space="preserve">pink</t>
   </si>
   <si>
+    <t xml:space="preserve">plum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alabama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purple</t>
+  </si>
+  <si>
     <t xml:space="preserve">banana</t>
   </si>
   <si>
@@ -71,12 +104,36 @@
     <t xml:space="preserve">yellow</t>
   </si>
   <si>
+    <t xml:space="preserve">pineapple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green-yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tangerine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persimmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deep orange</t>
+  </si>
+  <si>
     <t xml:space="preserve">coconut</t>
   </si>
   <si>
-    <t xml:space="preserve">Hawaii</t>
-  </si>
-  <si>
     <t xml:space="preserve">brown</t>
   </si>
   <si>
@@ -95,25 +152,31 @@
     <t xml:space="preserve">Shape</t>
   </si>
   <si>
+    <t xml:space="preserve">roundish</t>
+  </si>
+  <si>
     <t xml:space="preserve">grapes</t>
   </si>
   <si>
     <t xml:space="preserve">pebbles</t>
   </si>
   <si>
-    <t xml:space="preserve">purple</t>
-  </si>
-  <si>
     <t xml:space="preserve">mango</t>
   </si>
   <si>
     <t xml:space="preserve">oval</t>
   </si>
   <si>
+    <t xml:space="preserve">round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spikey</t>
+  </si>
+  <si>
     <t xml:space="preserve">flat</t>
   </si>
   <si>
-    <t xml:space="preserve">orange</t>
+    <t xml:space="preserve">acorn</t>
   </si>
   <si>
     <t xml:space="preserve">elongated</t>
@@ -208,7 +271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -218,6 +281,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,10 +313,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -264,115 +331,227 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>44866</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>44867</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
+        <v>44866</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>44866</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>44867</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>44867</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>44868</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
         <v>44870</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>44870</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>44871</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>44872</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
         <v>44885</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B16" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
         <v>44886</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B17" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="4"/>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -390,17 +569,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,80 +587,175 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="4"/>
+      <c r="B16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>